<commit_message>
Add curriculum learning support and update training parameters in train.py
</commit_message>
<xml_diff>
--- a/Mesure.xlsx
+++ b/Mesure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\ENSIM\5A\DRL\Git\DeepRenforcementLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8056BB2D-56F5-4C77-8018-14F80454A6AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81042E90-056C-4F03-BD85-9D700FAD569F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0806FB1C-282D-4709-952F-DE4506AD4B4F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0806FB1C-282D-4709-952F-DE4506AD4B4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Level 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="107">
   <si>
     <t>Niveau 1</t>
   </si>
@@ -62,9 +62,6 @@
     <t>Method adaptation : CL</t>
   </si>
   <si>
-    <t>Method adaptation : Train Zero</t>
-  </si>
-  <si>
     <t>Ne pas refaire d'entrainement apres le niveau 1</t>
   </si>
   <si>
@@ -116,6 +113,9 @@
     <t>Commande</t>
   </si>
   <si>
+    <t>60.0%</t>
+  </si>
+  <si>
     <t>214.3 steps</t>
   </si>
   <si>
@@ -245,9 +245,6 @@
     <t>423.0 steps</t>
   </si>
   <si>
-    <t>python train.py -a ppo -s 1 --active_sheep -c models/ppo_sheep1_obst0_sleepy.zip</t>
-  </si>
-  <si>
     <t>Train Command</t>
   </si>
   <si>
@@ -269,7 +266,88 @@
     <t>1,325 hr</t>
   </si>
   <si>
-    <t>1,892 hr</t>
+    <t>python train.py -a ppo -s 1 --active_sheep -c models/ppo_sheep1_obst0_sleepy.zip -cl</t>
+  </si>
+  <si>
+    <t>Method adaptation : Scratch</t>
+  </si>
+  <si>
+    <t>python train.py -a td3 -s 1 --active_sheep -c models/td3_sheep1_obst0_sleepy.zip -cl</t>
+  </si>
+  <si>
+    <t>python train.py -a dqn -s 1 --active_sheep -c models/dqn_sheep1_obst0_sleepy_best.pth -cl</t>
+  </si>
+  <si>
+    <t>python test.py -t DQN -a models/dqn_sheep1_obst0_curriculum_best.pth -s 1 --active_sheep -n 100</t>
+  </si>
+  <si>
+    <t>python test.py -t TD3 -a models/td3_sheep1_obst0_curriculum.zip -s 1 --active_sheep -n 100</t>
+  </si>
+  <si>
+    <t>python test.py -t PPO -a models/ppo_sheep1_obst0_curriculum.zip -s 1 --active_sheep -n 100</t>
+  </si>
+  <si>
+    <t>python train.py -a ppo -s 1 --active_sheep</t>
+  </si>
+  <si>
+    <t>python train.py -a td3 -s 1 --active_sheep</t>
+  </si>
+  <si>
+    <t>python train.py -a dqn -s 1 --active_sheep</t>
+  </si>
+  <si>
+    <t>python test.py -t PPO -a models/ppo_sheep1_obst0_active.zip -s 1 --active_sheep -n 100</t>
+  </si>
+  <si>
+    <t>python test.py -t TD3 -a models/td3_sheep1_obst0_active.zip -s 1 --active_sheep -n 100</t>
+  </si>
+  <si>
+    <t>python test.py -t DQN -a models/dqn_sheep1_obst0_active_best.pth -s 1 --active_sheep -n 100</t>
+  </si>
+  <si>
+    <t>1,067 hr</t>
+  </si>
+  <si>
+    <t>38,32 min</t>
+  </si>
+  <si>
+    <t>-9.87 ± 587.48</t>
+  </si>
+  <si>
+    <t>234.6 steps</t>
+  </si>
+  <si>
+    <t>-1074.19 ± 408.81</t>
+  </si>
+  <si>
+    <t>377.6 steps</t>
+  </si>
+  <si>
+    <t>29.0%</t>
+  </si>
+  <si>
+    <t>2,541 hr</t>
+  </si>
+  <si>
+    <t>1,134 hr</t>
+  </si>
+  <si>
+    <t>596.10 ± 474.32</t>
+  </si>
+  <si>
+    <t>56.0%</t>
+  </si>
+  <si>
+    <t>235.6 steps</t>
+  </si>
+  <si>
+    <t>-880.67 ± 414.22</t>
+  </si>
+  <si>
+    <t>27.0%</t>
+  </si>
+  <si>
+    <t>371.2 steps</t>
   </si>
 </sst>
 </file>
@@ -459,7 +537,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -565,6 +643,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -904,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0744EF66-6EF5-4E6D-8377-EBF08112D5D6}">
   <dimension ref="B2:Q11"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -925,14 +1006,14 @@
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
       <c r="K2" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L2" s="29"/>
       <c r="M2" s="29"/>
@@ -963,7 +1044,7 @@
     <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>30</v>
@@ -978,7 +1059,7 @@
         <v>59</v>
       </c>
       <c r="H5" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -995,7 +1076,7 @@
         <v>59</v>
       </c>
       <c r="Q5" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
@@ -1003,7 +1084,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>39</v>
@@ -1031,7 +1112,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>42</v>
@@ -1059,16 +1140,16 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="F8" s="16" t="s">
         <v>21</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>22</v>
       </c>
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
@@ -1087,7 +1168,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>45</v>
@@ -1099,10 +1180,10 @@
         <v>29</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>4</v>
@@ -1119,7 +1200,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>33</v>
@@ -1131,10 +1212,10 @@
         <v>35</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>5</v>
@@ -1151,7 +1232,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>36</v>
@@ -1163,10 +1244,10 @@
         <v>38</v>
       </c>
       <c r="G11" s="37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K11" s="14" t="s">
         <v>6</v>
@@ -1191,21 +1272,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F0C723-653A-4E8B-BD64-04ABCDEBBBC0}">
-  <dimension ref="B2:Q31"/>
+  <dimension ref="B2:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="87" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="90.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="29.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -1217,14 +1298,14 @@
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
       <c r="K2" s="29" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L2" s="29"/>
       <c r="M2" s="29"/>
@@ -1232,7 +1313,7 @@
       <c r="O2" s="29"/>
     </row>
     <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:17" ht="24.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:17" ht="24" x14ac:dyDescent="0.4">
       <c r="B4" s="1"/>
       <c r="C4" s="17" t="s">
         <v>7</v>
@@ -1243,7 +1324,7 @@
       <c r="E4" s="27"/>
       <c r="F4" s="28"/>
       <c r="H4" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I4" s="18"/>
       <c r="K4" s="1"/>
@@ -1256,7 +1337,7 @@
       <c r="N4" s="27"/>
       <c r="O4" s="28"/>
       <c r="Q4" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1273,9 +1354,7 @@
       <c r="F5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="38" t="s">
-        <v>59</v>
-      </c>
+      <c r="G5" s="33"/>
       <c r="H5" s="20"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
@@ -1290,9 +1369,7 @@
       <c r="O5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="P5" s="38" t="s">
-        <v>59</v>
-      </c>
+      <c r="P5" s="33"/>
       <c r="Q5" s="33"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
@@ -1311,7 +1388,7 @@
       <c r="F6" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="35"/>
+      <c r="G6" s="39"/>
       <c r="H6" s="20"/>
       <c r="K6" s="3" t="s">
         <v>1</v>
@@ -1320,7 +1397,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="6"/>
       <c r="O6" s="7"/>
-      <c r="P6" s="35"/>
+      <c r="P6" s="39"/>
       <c r="Q6" s="39"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
@@ -1333,22 +1410,22 @@
       <c r="D7" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="41" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="35"/>
+      <c r="G7" s="39"/>
       <c r="H7" s="20"/>
       <c r="K7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="9"/>
-      <c r="N7" s="10"/>
+      <c r="N7" s="41"/>
       <c r="O7" s="11"/>
-      <c r="P7" s="35"/>
+      <c r="P7" s="39"/>
       <c r="Q7" s="39"/>
     </row>
     <row r="8" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1367,7 +1444,7 @@
       <c r="F8" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="G8" s="35"/>
+      <c r="G8" s="39"/>
       <c r="H8" s="20"/>
       <c r="K8" s="8" t="s">
         <v>3</v>
@@ -1376,7 +1453,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="12"/>
       <c r="O8" s="13"/>
-      <c r="P8" s="35"/>
+      <c r="P8" s="39"/>
       <c r="Q8" s="39"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
@@ -1389,22 +1466,22 @@
       <c r="D9" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="G9" s="34"/>
+      <c r="G9" s="33"/>
       <c r="H9" s="20"/>
       <c r="K9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="9"/>
-      <c r="N9" s="10"/>
+      <c r="N9" s="41"/>
       <c r="O9" s="11"/>
-      <c r="P9" s="34"/>
+      <c r="P9" s="33"/>
       <c r="Q9" s="40"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
@@ -1417,22 +1494,22 @@
       <c r="D10" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="36"/>
+      <c r="G10" s="33"/>
       <c r="H10" s="20"/>
       <c r="K10" s="8" t="s">
         <v>6</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="10"/>
+      <c r="N10" s="41"/>
       <c r="O10" s="11"/>
-      <c r="P10" s="36"/>
+      <c r="P10" s="33"/>
       <c r="Q10" s="40"/>
     </row>
     <row r="11" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1448,10 +1525,10 @@
       <c r="E11" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="37"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="20"/>
       <c r="K11" s="14" t="s">
         <v>4</v>
@@ -1460,14 +1537,20 @@
       <c r="M11" s="2"/>
       <c r="N11" s="12"/>
       <c r="O11" s="13"/>
-      <c r="P11" s="37"/>
+      <c r="P11" s="33"/>
       <c r="Q11" s="40"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="H12" s="20"/>
       <c r="Q12" s="20"/>
     </row>
     <row r="13" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
       <c r="H13" s="20"/>
       <c r="Q13" s="20"/>
     </row>
@@ -1482,7 +1565,7 @@
       <c r="E14" s="27"/>
       <c r="F14" s="28"/>
       <c r="H14" s="21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="17" t="s">
@@ -1494,7 +1577,7 @@
       <c r="N14" s="31"/>
       <c r="O14" s="32"/>
       <c r="Q14" s="21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1515,7 +1598,7 @@
         <v>59</v>
       </c>
       <c r="H15" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
@@ -1534,7 +1617,7 @@
         <v>59</v>
       </c>
       <c r="Q15" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
@@ -1544,7 +1627,7 @@
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
+      <c r="F16" s="22"/>
       <c r="G16" s="35"/>
       <c r="H16" s="35"/>
       <c r="K16" s="3" t="s">
@@ -1564,7 +1647,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
+      <c r="F17" s="23"/>
       <c r="G17" s="35"/>
       <c r="H17" s="35"/>
       <c r="K17" s="8" t="s">
@@ -1584,7 +1667,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
+      <c r="F18" s="16"/>
       <c r="G18" s="35"/>
       <c r="H18" s="35"/>
       <c r="K18" s="8" t="s">
@@ -1601,15 +1684,23 @@
       <c r="B19" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
+      <c r="C19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>95</v>
+      </c>
       <c r="G19" s="34" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>5</v>
@@ -1625,12 +1716,16 @@
       <c r="B20" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
+      <c r="F20" s="23"/>
       <c r="G20" s="36"/>
-      <c r="H20" s="8"/>
+      <c r="H20" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="K20" s="8" t="s">
         <v>6</v>
       </c>
@@ -1645,12 +1740,24 @@
       <c r="B21" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="14"/>
+      <c r="C21" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="H21" s="14" t="s">
+        <v>82</v>
+      </c>
       <c r="K21" s="14" t="s">
         <v>4</v>
       </c>
@@ -1662,10 +1769,16 @@
       <c r="Q21" s="14"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
       <c r="H22" s="20"/>
       <c r="Q22" s="20"/>
     </row>
     <row r="23" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
       <c r="H23" s="20"/>
       <c r="Q23" s="20"/>
     </row>
@@ -1680,7 +1793,7 @@
       <c r="E24" s="27"/>
       <c r="F24" s="28"/>
       <c r="H24" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="17" t="s">
@@ -1692,13 +1805,13 @@
       <c r="N24" s="27"/>
       <c r="O24" s="28"/>
       <c r="Q24" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>30</v>
@@ -1713,11 +1826,11 @@
         <v>59</v>
       </c>
       <c r="H25" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>30</v>
@@ -1732,7 +1845,7 @@
         <v>59</v>
       </c>
       <c r="Q25" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
@@ -1742,7 +1855,7 @@
       <c r="C26" s="4"/>
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
-      <c r="F26" s="7"/>
+      <c r="F26" s="22"/>
       <c r="G26" s="35"/>
       <c r="H26" s="35"/>
       <c r="K26" s="3" t="s">
@@ -1762,7 +1875,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="9"/>
       <c r="E27" s="10"/>
-      <c r="F27" s="11"/>
+      <c r="F27" s="23"/>
       <c r="G27" s="35"/>
       <c r="H27" s="35"/>
       <c r="K27" s="8" t="s">
@@ -1782,7 +1895,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
       <c r="E28" s="12"/>
-      <c r="F28" s="13"/>
+      <c r="F28" s="16"/>
       <c r="G28" s="35"/>
       <c r="H28" s="35"/>
       <c r="K28" s="8" t="s">
@@ -1799,12 +1912,24 @@
       <c r="B29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="34"/>
-      <c r="H29" s="3"/>
+      <c r="C29" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="G29" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="K29" s="3" t="s">
         <v>5</v>
       </c>
@@ -1819,12 +1944,16 @@
       <c r="B30" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="D30" s="9"/>
       <c r="E30" s="10"/>
-      <c r="F30" s="11"/>
+      <c r="F30" s="23"/>
       <c r="G30" s="36"/>
-      <c r="H30" s="8"/>
+      <c r="H30" s="8" t="s">
+        <v>87</v>
+      </c>
       <c r="K30" s="8" t="s">
         <v>6</v>
       </c>
@@ -1839,12 +1968,24 @@
       <c r="B31" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="14"/>
+      <c r="C31" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>88</v>
+      </c>
       <c r="K31" s="14" t="s">
         <v>4</v>
       </c>
@@ -1854,6 +1995,11 @@
       <c r="O31" s="13"/>
       <c r="P31" s="37"/>
       <c r="Q31" s="14"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1874,8 +2020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD226A34-13FF-4F4D-A688-C597425C2EF8}">
   <dimension ref="B2:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25:Q31"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1898,14 +2044,14 @@
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" s="29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
       <c r="K2" s="29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L2" s="29"/>
       <c r="M2" s="29"/>
@@ -1913,30 +2059,30 @@
       <c r="O2" s="29"/>
     </row>
     <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:17" ht="24.75" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:17" ht="24" x14ac:dyDescent="0.4">
       <c r="B4" s="1"/>
       <c r="C4" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" s="27"/>
       <c r="F4" s="28"/>
       <c r="H4" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="17" t="s">
         <v>7</v>
       </c>
       <c r="M4" s="26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N4" s="27"/>
       <c r="O4" s="28"/>
       <c r="Q4" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1953,9 +2099,7 @@
       <c r="F5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="38" t="s">
-        <v>59</v>
-      </c>
+      <c r="G5" s="33"/>
       <c r="H5" s="20"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1" t="s">
@@ -1970,9 +2114,7 @@
       <c r="O5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="P5" s="38" t="s">
-        <v>59</v>
-      </c>
+      <c r="P5" s="33"/>
       <c r="Q5" s="20"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
@@ -1983,7 +2125,7 @@
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="35"/>
+      <c r="G6" s="39"/>
       <c r="H6" s="20"/>
       <c r="K6" s="3" t="s">
         <v>1</v>
@@ -1992,7 +2134,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="6"/>
       <c r="O6" s="7"/>
-      <c r="P6" s="35"/>
+      <c r="P6" s="39"/>
       <c r="Q6" s="20"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
@@ -2001,18 +2143,18 @@
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="11"/>
-      <c r="G7" s="35"/>
+      <c r="G7" s="39"/>
       <c r="H7" s="20"/>
       <c r="K7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="9"/>
-      <c r="N7" s="10"/>
+      <c r="N7" s="41"/>
       <c r="O7" s="11"/>
-      <c r="P7" s="35"/>
+      <c r="P7" s="39"/>
       <c r="Q7" s="20"/>
     </row>
     <row r="8" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2023,7 +2165,7 @@
       <c r="D8" s="2"/>
       <c r="E8" s="12"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="35"/>
+      <c r="G8" s="39"/>
       <c r="H8" s="20"/>
       <c r="K8" s="8" t="s">
         <v>3</v>
@@ -2032,7 +2174,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="12"/>
       <c r="O8" s="13"/>
-      <c r="P8" s="35"/>
+      <c r="P8" s="39"/>
       <c r="Q8" s="20"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
@@ -2041,18 +2183,18 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
+      <c r="E9" s="41"/>
       <c r="F9" s="11"/>
-      <c r="G9" s="34"/>
+      <c r="G9" s="33"/>
       <c r="H9" s="20"/>
       <c r="K9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="9"/>
-      <c r="N9" s="10"/>
+      <c r="N9" s="41"/>
       <c r="O9" s="11"/>
-      <c r="P9" s="34"/>
+      <c r="P9" s="33"/>
       <c r="Q9" s="20"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
@@ -2061,18 +2203,18 @@
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
+      <c r="E10" s="41"/>
       <c r="F10" s="11"/>
-      <c r="G10" s="36"/>
+      <c r="G10" s="33"/>
       <c r="H10" s="20"/>
       <c r="K10" s="8" t="s">
         <v>6</v>
       </c>
       <c r="L10" s="1"/>
       <c r="M10" s="9"/>
-      <c r="N10" s="10"/>
+      <c r="N10" s="41"/>
       <c r="O10" s="11"/>
-      <c r="P10" s="36"/>
+      <c r="P10" s="33"/>
       <c r="Q10" s="20"/>
     </row>
     <row r="11" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2083,7 +2225,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="37"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="20"/>
       <c r="K11" s="14" t="s">
         <v>4</v>
@@ -2092,7 +2234,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="12"/>
       <c r="O11" s="13"/>
-      <c r="P11" s="37"/>
+      <c r="P11" s="33"/>
       <c r="Q11" s="20"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
@@ -2109,24 +2251,24 @@
         <v>7</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" s="27"/>
       <c r="F14" s="28"/>
       <c r="H14" s="21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K14" s="1"/>
       <c r="L14" s="17" t="s">
         <v>7</v>
       </c>
       <c r="M14" s="26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N14" s="27"/>
       <c r="O14" s="28"/>
       <c r="Q14" s="21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2147,7 +2289,7 @@
         <v>59</v>
       </c>
       <c r="H15" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
@@ -2166,7 +2308,7 @@
         <v>59</v>
       </c>
       <c r="Q15" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
@@ -2303,30 +2445,30 @@
         <v>7</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E24" s="27"/>
       <c r="F24" s="28"/>
       <c r="H24" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K24" s="1"/>
       <c r="L24" s="17" t="s">
         <v>7</v>
       </c>
       <c r="M24" s="26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N24" s="27"/>
       <c r="O24" s="28"/>
       <c r="Q24" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>30</v>
@@ -2341,11 +2483,11 @@
         <v>59</v>
       </c>
       <c r="H25" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>30</v>
@@ -2360,7 +2502,7 @@
         <v>59</v>
       </c>
       <c r="Q25" s="38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add new model files and log events for DQN and PPO training experiments
</commit_message>
<xml_diff>
--- a/Mesure.xlsx
+++ b/Mesure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\ENSIM\5A\DRL\Git\DeepRenforcementLearning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81042E90-056C-4F03-BD85-9D700FAD569F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA8E0AE-CCAF-48D7-A90F-AA55CB5F83B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0806FB1C-282D-4709-952F-DE4506AD4B4F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{0806FB1C-282D-4709-952F-DE4506AD4B4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Level 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="110">
   <si>
     <t>Niveau 1</t>
   </si>
@@ -348,6 +348,15 @@
   </si>
   <si>
     <t>371.2 steps</t>
+  </si>
+  <si>
+    <t>python test.py -t lazy -s 1 -r 0.2 --active_sheep -n 100</t>
+  </si>
+  <si>
+    <t>-3502.87 ± 501.03</t>
+  </si>
+  <si>
+    <t>422.8 steps</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1283,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F0C723-653A-4E8B-BD64-04ABCDEBBBC0}">
   <dimension ref="B2:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -2018,17 +2027,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD226A34-13FF-4F4D-A688-C597425C2EF8}">
-  <dimension ref="B2:Q31"/>
+  <dimension ref="B2:Q32"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -2121,10 +2130,18 @@
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="7"/>
+      <c r="C6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>109</v>
+      </c>
       <c r="G6" s="39"/>
       <c r="H6" s="20"/>
       <c r="K6" s="3" t="s">
@@ -2144,7 +2161,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="9"/>
       <c r="E7" s="41"/>
-      <c r="F7" s="11"/>
+      <c r="F7" s="23"/>
       <c r="G7" s="39"/>
       <c r="H7" s="20"/>
       <c r="K7" s="8" t="s">
@@ -2164,7 +2181,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
       <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
+      <c r="F8" s="16"/>
       <c r="G8" s="39"/>
       <c r="H8" s="20"/>
       <c r="K8" s="8" t="s">
@@ -2184,7 +2201,7 @@
       <c r="C9" s="4"/>
       <c r="D9" s="9"/>
       <c r="E9" s="41"/>
-      <c r="F9" s="11"/>
+      <c r="F9" s="23"/>
       <c r="G9" s="33"/>
       <c r="H9" s="20"/>
       <c r="K9" s="3" t="s">
@@ -2204,7 +2221,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="9"/>
       <c r="E10" s="41"/>
-      <c r="F10" s="11"/>
+      <c r="F10" s="23"/>
       <c r="G10" s="33"/>
       <c r="H10" s="20"/>
       <c r="K10" s="8" t="s">
@@ -2224,7 +2241,7 @@
       <c r="C11" s="15"/>
       <c r="D11" s="2"/>
       <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
+      <c r="F11" s="16"/>
       <c r="G11" s="33"/>
       <c r="H11" s="20"/>
       <c r="K11" s="14" t="s">
@@ -2238,10 +2255,16 @@
       <c r="Q11" s="20"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="H12" s="20"/>
       <c r="Q12" s="20"/>
     </row>
     <row r="13" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
       <c r="H13" s="20"/>
       <c r="Q13" s="20"/>
     </row>
@@ -2318,7 +2341,7 @@
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="7"/>
+      <c r="F16" s="22"/>
       <c r="G16" s="35"/>
       <c r="H16" s="35"/>
       <c r="K16" s="3" t="s">
@@ -2338,7 +2361,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
+      <c r="F17" s="23"/>
       <c r="G17" s="35"/>
       <c r="H17" s="35"/>
       <c r="K17" s="8" t="s">
@@ -2358,7 +2381,7 @@
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
       <c r="E18" s="12"/>
-      <c r="F18" s="13"/>
+      <c r="F18" s="16"/>
       <c r="G18" s="35"/>
       <c r="H18" s="35"/>
       <c r="K18" s="8" t="s">
@@ -2378,7 +2401,7 @@
       <c r="C19" s="4"/>
       <c r="D19" s="9"/>
       <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
+      <c r="F19" s="23"/>
       <c r="G19" s="34"/>
       <c r="H19" s="3"/>
       <c r="K19" s="3" t="s">
@@ -2398,7 +2421,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
+      <c r="F20" s="23"/>
       <c r="G20" s="36"/>
       <c r="H20" s="8"/>
       <c r="K20" s="8" t="s">
@@ -2418,7 +2441,7 @@
       <c r="C21" s="15"/>
       <c r="D21" s="2"/>
       <c r="E21" s="12"/>
-      <c r="F21" s="13"/>
+      <c r="F21" s="16"/>
       <c r="G21" s="37"/>
       <c r="H21" s="14"/>
       <c r="K21" s="14" t="s">
@@ -2432,10 +2455,16 @@
       <c r="Q21" s="14"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
       <c r="H22" s="20"/>
       <c r="Q22" s="20"/>
     </row>
     <row r="23" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
       <c r="H23" s="20"/>
       <c r="Q23" s="20"/>
     </row>
@@ -2512,7 +2541,7 @@
       <c r="C26" s="4"/>
       <c r="D26" s="5"/>
       <c r="E26" s="6"/>
-      <c r="F26" s="7"/>
+      <c r="F26" s="22"/>
       <c r="G26" s="35"/>
       <c r="H26" s="35"/>
       <c r="K26" s="3" t="s">
@@ -2532,7 +2561,7 @@
       <c r="C27" s="1"/>
       <c r="D27" s="9"/>
       <c r="E27" s="10"/>
-      <c r="F27" s="11"/>
+      <c r="F27" s="23"/>
       <c r="G27" s="35"/>
       <c r="H27" s="35"/>
       <c r="K27" s="8" t="s">
@@ -2552,7 +2581,7 @@
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
       <c r="E28" s="12"/>
-      <c r="F28" s="13"/>
+      <c r="F28" s="16"/>
       <c r="G28" s="35"/>
       <c r="H28" s="35"/>
       <c r="K28" s="8" t="s">
@@ -2572,7 +2601,7 @@
       <c r="C29" s="4"/>
       <c r="D29" s="9"/>
       <c r="E29" s="10"/>
-      <c r="F29" s="11"/>
+      <c r="F29" s="23"/>
       <c r="G29" s="34"/>
       <c r="H29" s="3"/>
       <c r="K29" s="3" t="s">
@@ -2592,7 +2621,7 @@
       <c r="C30" s="1"/>
       <c r="D30" s="9"/>
       <c r="E30" s="10"/>
-      <c r="F30" s="11"/>
+      <c r="F30" s="23"/>
       <c r="G30" s="36"/>
       <c r="H30" s="8"/>
       <c r="K30" s="8" t="s">
@@ -2612,7 +2641,7 @@
       <c r="C31" s="15"/>
       <c r="D31" s="2"/>
       <c r="E31" s="12"/>
-      <c r="F31" s="13"/>
+      <c r="F31" s="16"/>
       <c r="G31" s="37"/>
       <c r="H31" s="14"/>
       <c r="K31" s="14" t="s">
@@ -2624,6 +2653,11 @@
       <c r="O31" s="13"/>
       <c r="P31" s="37"/>
       <c r="Q31" s="14"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>